<commit_message>
Se agrego la funcionalidad de leer el documento, la clase lista y archivo
</commit_message>
<xml_diff>
--- a/CVSReader/src/Docs/Lista.xlsx
+++ b/CVSReader/src/Docs/Lista.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos\Semestre 4\Diseño de software\Unidad 1\ADA3\CVSReader\src\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D31B8729-DB4D-4C0C-AD9D-153D79945ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A519CA3E-A945-4DBE-BEF2-39785D4495EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="1" r:id="rId1"/>

</xml_diff>